<commit_message>
commiting module 3 assignments and module 5 directory
</commit_message>
<xml_diff>
--- a/fall24/csd310/Module-3/normalization.xlsx
+++ b/fall24/csd310/Module-3/normalization.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paul/Developer/school/fall24/csd310/Module-3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4761CE5-C278-284A-937F-CE3A0F2FCF09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10BA1B7D-4BA4-6244-B5CE-6A881AAFBD7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{04C407C8-F15E-E84E-A22F-A0C3025438E0}"/>
+    <workbookView xWindow="160" yWindow="920" windowWidth="29920" windowHeight="18560" xr2:uid="{04C407C8-F15E-E84E-A22F-A0C3025438E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
   <si>
     <t>publisher_name</t>
   </si>
@@ -84,13 +84,37 @@
   </si>
   <si>
     <t>CSD310</t>
+  </si>
+  <si>
+    <t>3NF</t>
+  </si>
+  <si>
+    <t>Publisher Table</t>
+  </si>
+  <si>
+    <t>Book Table</t>
+  </si>
+  <si>
+    <t>Author Table</t>
+  </si>
+  <si>
+    <t>author_id</t>
+  </si>
+  <si>
+    <t>publisher_id</t>
+  </si>
+  <si>
+    <t>Primary Key</t>
+  </si>
+  <si>
+    <t>Foreign Key</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -104,13 +128,32 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -125,9 +168,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,22 +511,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{177129FE-79E2-3B44-9780-4AB90F4CBC97}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
   </cols>
@@ -492,6 +542,9 @@
       <c r="D1" t="s">
         <v>15</v>
       </c>
+      <c r="E1" s="2">
+        <v>45533</v>
+      </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -500,39 +553,120 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="1" t="s">
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K10" s="3"/>
+      <c r="L10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="K11" s="4"/>
+      <c r="L11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>